<commit_message>
uploaded reviewed DE excel files
</commit_message>
<xml_diff>
--- a/default-mappings-xlsx/visitreport/VisitReport_Mapping_MSDynamics_DE.xlsx
+++ b/default-mappings-xlsx/visitreport/VisitReport_Mapping_MSDynamics_DE.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcusKlapprodt\snapADDY GmbH\Sebastian Metzger - Mapping\2_Vorlagen CRM Mapping\VisitReport\2019\DE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="14_{E7E331D1-8E9B-47B4-AC6C-2D8272A0A12F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{03E4A0F4-0CCE-49ED-9D67-940F95571352}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="14_{E7E331D1-8E9B-47B4-AC6C-2D8272A0A12F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0F403604-52CA-469A-8A5B-D182CB5B0376}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specifications" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Field_type">Specifications!$I$7:$I$24,Specifications!$M$7:$M$24,Specifications!$Q$7:$Q$24,Specifications!$U$7:$U$24,Specifications!$Y$7:$Y$24,Specifications!$Y$28:$Y$37,Specifications!$U$28:$U$37,Specifications!$Q$28:$Q$37,Specifications!$M$28:$M$37,Specifications!$I$28:$I$37,Specifications!$I$39:$I$48,Specifications!$Q$39:$Q$48,Specifications!$U$39:$U$48,Specifications!$Y$39:$Y$48,Specifications!$Y$51:$Y$61,Specifications!$U$51:$U$61,Specifications!$Q$51:$Q$61,Specifications!$M$51:$M$61,Specifications!$I$51:$I$61,Specifications!$M$39:$M$48</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="98">
   <si>
     <t>Website</t>
   </si>
@@ -42,12 +45,6 @@
     <t>Fax</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Dropdown</t>
-  </si>
-  <si>
     <t>Salutation</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>not used</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>"snapADDY"</t>
   </si>
   <si>
@@ -201,9 +195,6 @@
     <t>Default Value</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>CRM System: MS Dynamics</t>
   </si>
   <si>
@@ -262,15 +253,6 @@
   </si>
   <si>
     <t>Geschlecht</t>
-  </si>
-  <si>
-    <t>nicht benötigt</t>
-  </si>
-  <si>
-    <t>muss ausgefüllt sein</t>
-  </si>
-  <si>
-    <t>andere Bemerkungen</t>
   </si>
   <si>
     <t>Frage 1 : z.B. Branche</t>
@@ -367,6 +349,15 @@
       </rPr>
       <t>[Hier bitte Namen der Master-Vorlage einfügen]</t>
     </r>
+  </si>
+  <si>
+    <t>mögl. Notizen</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>number</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1774,9 +1765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
@@ -1823,6 +1812,34 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1862,39 +1879,33 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.1498764000366222"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2189,18 +2200,18 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="snapADDY" pivot="0" count="5" xr9:uid="{A8851A67-88BF-475D-B211-A3CFCBFE5DEE}">
-      <tableStyleElement type="wholeTable" dxfId="24"/>
-      <tableStyleElement type="headerRow" dxfId="23"/>
-      <tableStyleElement type="firstColumn" dxfId="22"/>
-      <tableStyleElement type="firstRowStripe" dxfId="21"/>
-      <tableStyleElement type="secondRowStripe" dxfId="20"/>
+      <tableStyleElement type="wholeTable" dxfId="26"/>
+      <tableStyleElement type="headerRow" dxfId="25"/>
+      <tableStyleElement type="firstColumn" dxfId="24"/>
+      <tableStyleElement type="firstRowStripe" dxfId="23"/>
+      <tableStyleElement type="secondRowStripe" dxfId="22"/>
     </tableStyle>
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF9DA600"/>
       <color rgb="FFB4C6E7"/>
       <color rgb="FF001E51"/>
-      <color rgb="FF9DA600"/>
       <color rgb="FFFE6C36"/>
       <color rgb="FFFEFFE1"/>
     </mruColors>
@@ -2824,32 +2835,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5027446F-BBDF-4A57-AA45-BC7D0EB64201}">
   <dimension ref="A1:Y62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.88671875" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="1.6640625" customWidth="1"/>
     <col min="7" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="1.7109375" customWidth="1"/>
+    <col min="10" max="10" width="1.6640625" customWidth="1"/>
     <col min="11" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="1.7109375" customWidth="1"/>
+    <col min="14" max="14" width="1.6640625" customWidth="1"/>
     <col min="15" max="17" width="15" customWidth="1"/>
-    <col min="18" max="18" width="1.7109375" customWidth="1"/>
+    <col min="18" max="18" width="1.6640625" customWidth="1"/>
     <col min="19" max="21" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="1.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="1.5546875" customWidth="1" outlineLevel="1"/>
     <col min="23" max="25" width="15" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="142" t="s">
-        <v>101</v>
+    <row r="1" spans="1:25" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="118" t="s">
+        <v>94</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2858,9 +2869,9 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2869,111 +2880,111 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:25" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G3" s="59"/>
       <c r="K3" s="59"/>
     </row>
-    <row r="4" spans="1:25" ht="63" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="61.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" s="40"/>
-      <c r="G4" s="129" t="s">
+      <c r="G4" s="137" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="137" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="137"/>
+      <c r="M4" s="137"/>
+      <c r="O4" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="137"/>
+      <c r="Q4" s="137"/>
+      <c r="S4" s="128" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="129"/>
+      <c r="U4" s="130"/>
+      <c r="W4" s="134" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="129"/>
-      <c r="I4" s="129"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="129" t="s">
-        <v>59</v>
-      </c>
-      <c r="L4" s="129"/>
-      <c r="M4" s="129"/>
-      <c r="O4" s="129" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" s="129"/>
-      <c r="Q4" s="129"/>
-      <c r="S4" s="120" t="s">
-        <v>63</v>
-      </c>
-      <c r="T4" s="121"/>
-      <c r="U4" s="122"/>
-      <c r="W4" s="126" t="s">
-        <v>62</v>
-      </c>
-      <c r="X4" s="127"/>
-      <c r="Y4" s="128"/>
-    </row>
-    <row r="5" spans="1:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X4" s="135"/>
+      <c r="Y4" s="136"/>
+    </row>
+    <row r="5" spans="1:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="51" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="67"/>
       <c r="C6" s="68"/>
       <c r="D6" s="68"/>
       <c r="E6" s="50" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G6" s="69" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H6" s="70" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I6" s="71" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="69" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L6" s="70" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M6" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="O6" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="70" t="s">
-        <v>32</v>
-      </c>
       <c r="Q6" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" s="93" t="s">
+        <v>27</v>
+      </c>
+      <c r="T6" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="S6" s="95" t="s">
-        <v>29</v>
-      </c>
-      <c r="T6" s="96" t="s">
-        <v>32</v>
-      </c>
-      <c r="U6" s="97" t="s">
+      <c r="U6" s="95" t="s">
+        <v>28</v>
+      </c>
+      <c r="W6" s="93" t="s">
+        <v>27</v>
+      </c>
+      <c r="X6" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="W6" s="95" t="s">
-        <v>29</v>
-      </c>
-      <c r="X6" s="96" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y6" s="97" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Y6" s="95" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="20"/>
-      <c r="C7" s="113"/>
+      <c r="C7" s="111"/>
       <c r="D7" s="25"/>
       <c r="E7" s="47"/>
       <c r="G7" s="72"/>
@@ -2986,543 +2997,535 @@
       <c r="O7" s="72"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="73"/>
-      <c r="S7" s="98"/>
+      <c r="S7" s="96"/>
       <c r="T7" s="6"/>
-      <c r="U7" s="99"/>
-      <c r="W7" s="98"/>
+      <c r="U7" s="97"/>
+      <c r="W7" s="96"/>
       <c r="X7" s="6"/>
-      <c r="Y7" s="99"/>
-    </row>
-    <row r="8" spans="1:25" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y7" s="97"/>
+    </row>
+    <row r="8" spans="1:25" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="60" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="114"/>
-      <c r="D8" s="62" t="s">
-        <v>51</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C8" s="112"/>
+      <c r="D8" s="62"/>
       <c r="E8" s="63"/>
       <c r="G8" s="74" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H8" s="64"/>
       <c r="I8" s="75" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="J8" s="65"/>
       <c r="K8" s="74" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L8" s="64"/>
       <c r="M8" s="75" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="O8" s="74"/>
       <c r="P8" s="64"/>
       <c r="Q8" s="75"/>
-      <c r="S8" s="100" t="s">
-        <v>44</v>
+      <c r="S8" s="98" t="s">
+        <v>42</v>
       </c>
       <c r="T8" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="U8" s="101"/>
-      <c r="W8" s="100"/>
+        <v>43</v>
+      </c>
+      <c r="U8" s="99" t="s">
+        <v>96</v>
+      </c>
+      <c r="W8" s="98"/>
       <c r="X8" s="64"/>
-      <c r="Y8" s="101"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y8" s="99"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="115" t="s">
-        <v>51</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="113"/>
       <c r="D9" s="26"/>
       <c r="E9" s="48"/>
       <c r="G9" s="76" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="76" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="O9" s="76"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="77"/>
-      <c r="S9" s="102" t="s">
-        <v>46</v>
+      <c r="S9" s="100" t="s">
+        <v>44</v>
       </c>
       <c r="T9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="U9" s="103"/>
-      <c r="W9" s="104"/>
+        <v>45</v>
+      </c>
+      <c r="U9" s="101" t="s">
+        <v>97</v>
+      </c>
+      <c r="W9" s="102"/>
       <c r="X9" s="5"/>
-      <c r="Y9" s="103"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y9" s="101"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="115" t="s">
-        <v>51</v>
-      </c>
+      <c r="C10" s="113"/>
       <c r="D10" s="26"/>
       <c r="E10" s="48"/>
       <c r="G10" s="76" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="76" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="O10" s="76"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="77"/>
-      <c r="S10" s="104"/>
+      <c r="S10" s="102"/>
       <c r="T10" s="5"/>
-      <c r="U10" s="103"/>
-      <c r="W10" s="104"/>
+      <c r="U10" s="101"/>
+      <c r="W10" s="102"/>
       <c r="X10" s="5"/>
-      <c r="Y10" s="103"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y10" s="101"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B11" s="21"/>
-      <c r="C11" s="115" t="s">
-        <v>51</v>
-      </c>
+      <c r="C11" s="113"/>
       <c r="D11" s="26"/>
       <c r="E11" s="48"/>
       <c r="G11" s="76" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="76" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="O11" s="76"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="77"/>
-      <c r="S11" s="104"/>
+      <c r="S11" s="102"/>
       <c r="T11" s="5"/>
-      <c r="U11" s="103"/>
-      <c r="W11" s="104"/>
+      <c r="U11" s="101"/>
+      <c r="W11" s="102"/>
       <c r="X11" s="5"/>
-      <c r="Y11" s="103"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y11" s="101"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="115"/>
+        <v>64</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="113"/>
       <c r="D12" s="26"/>
       <c r="E12" s="48"/>
       <c r="G12" s="76" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="76"/>
       <c r="L12" s="5"/>
       <c r="M12" s="77"/>
       <c r="O12" s="76" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P12" s="5"/>
       <c r="Q12" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="S12" s="104"/>
+        <v>39</v>
+      </c>
+      <c r="S12" s="102"/>
       <c r="T12" s="5"/>
-      <c r="U12" s="103"/>
-      <c r="W12" s="104"/>
+      <c r="U12" s="101"/>
+      <c r="W12" s="102"/>
       <c r="X12" s="5"/>
-      <c r="Y12" s="103"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y12" s="101"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="22"/>
-      <c r="C13" s="115"/>
+      <c r="C13" s="113"/>
       <c r="D13" s="26"/>
       <c r="E13" s="48"/>
       <c r="G13" s="72" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H13" s="6"/>
-      <c r="I13" s="73" t="s">
-        <v>3</v>
+      <c r="I13" s="77" t="s">
+        <v>39</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="72" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L13" s="6"/>
-      <c r="M13" s="73" t="s">
-        <v>3</v>
+      <c r="M13" s="77" t="s">
+        <v>39</v>
       </c>
       <c r="O13" s="72" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P13" s="6"/>
-      <c r="Q13" s="73" t="s">
-        <v>3</v>
-      </c>
-      <c r="S13" s="104"/>
+      <c r="Q13" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="S13" s="102"/>
       <c r="T13" s="5"/>
-      <c r="U13" s="103"/>
-      <c r="W13" s="104"/>
+      <c r="U13" s="101"/>
+      <c r="W13" s="102"/>
       <c r="X13" s="5"/>
-      <c r="Y13" s="103"/>
-    </row>
-    <row r="14" spans="1:25" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y13" s="101"/>
+    </row>
+    <row r="14" spans="1:25" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="60" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="61"/>
-      <c r="C14" s="114"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="62"/>
       <c r="E14" s="63"/>
       <c r="G14" s="78" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H14" s="66"/>
-      <c r="I14" s="79" t="s">
-        <v>3</v>
+      <c r="I14" s="77" t="s">
+        <v>39</v>
       </c>
       <c r="J14" s="65"/>
       <c r="K14" s="78" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L14" s="66"/>
-      <c r="M14" s="79" t="s">
-        <v>3</v>
+      <c r="M14" s="77" t="s">
+        <v>39</v>
       </c>
       <c r="O14" s="78" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P14" s="66"/>
-      <c r="Q14" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="S14" s="105"/>
+      <c r="Q14" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="S14" s="103"/>
       <c r="T14" s="66"/>
-      <c r="U14" s="106"/>
-      <c r="W14" s="105"/>
+      <c r="U14" s="104"/>
+      <c r="W14" s="103"/>
       <c r="X14" s="66"/>
-      <c r="Y14" s="106"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y14" s="104"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B15" s="23"/>
-      <c r="C15" s="115"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="26"/>
       <c r="E15" s="48"/>
-      <c r="G15" s="80" t="s">
-        <v>12</v>
+      <c r="G15" s="79" t="s">
+        <v>10</v>
       </c>
       <c r="H15" s="10"/>
-      <c r="I15" s="81" t="s">
-        <v>3</v>
+      <c r="I15" s="77" t="s">
+        <v>39</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="K15" s="80" t="s">
-        <v>20</v>
+      <c r="K15" s="79" t="s">
+        <v>18</v>
       </c>
       <c r="L15" s="10"/>
-      <c r="M15" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="O15" s="80" t="s">
-        <v>26</v>
+      <c r="M15" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="79" t="s">
+        <v>24</v>
       </c>
       <c r="P15" s="10"/>
-      <c r="Q15" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="S15" s="104"/>
+      <c r="Q15" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="S15" s="102"/>
       <c r="T15" s="5"/>
-      <c r="U15" s="103"/>
-      <c r="W15" s="104"/>
+      <c r="U15" s="101"/>
+      <c r="W15" s="102"/>
       <c r="X15" s="5"/>
-      <c r="Y15" s="103"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y15" s="101"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B16" s="21"/>
-      <c r="C16" s="115"/>
+      <c r="C16" s="113"/>
       <c r="D16" s="26"/>
       <c r="E16" s="48"/>
       <c r="G16" s="76" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="76" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="O16" s="76" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="P16" s="5"/>
       <c r="Q16" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="S16" s="104"/>
+        <v>39</v>
+      </c>
+      <c r="S16" s="102"/>
       <c r="T16" s="5"/>
-      <c r="U16" s="103"/>
-      <c r="W16" s="104"/>
+      <c r="U16" s="101"/>
+      <c r="W16" s="102"/>
       <c r="X16" s="5"/>
-      <c r="Y16" s="103"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y16" s="101"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="21"/>
-      <c r="C17" s="115"/>
+      <c r="C17" s="113"/>
       <c r="D17" s="26"/>
       <c r="E17" s="48"/>
       <c r="G17" s="76" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="76" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="O17" s="76" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P17" s="5"/>
       <c r="Q17" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="S17" s="104"/>
+        <v>39</v>
+      </c>
+      <c r="S17" s="102"/>
       <c r="T17" s="5"/>
-      <c r="U17" s="103"/>
-      <c r="W17" s="104"/>
+      <c r="U17" s="101"/>
+      <c r="W17" s="102"/>
       <c r="X17" s="5"/>
-      <c r="Y17" s="103"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y17" s="101"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B18" s="21"/>
-      <c r="C18" s="115"/>
+      <c r="C18" s="113"/>
       <c r="D18" s="26"/>
       <c r="E18" s="48"/>
       <c r="G18" s="76" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="76" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="O18" s="76" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="P18" s="5"/>
       <c r="Q18" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="S18" s="104"/>
+        <v>39</v>
+      </c>
+      <c r="S18" s="102"/>
       <c r="T18" s="5"/>
-      <c r="U18" s="103"/>
-      <c r="W18" s="104"/>
+      <c r="U18" s="101"/>
+      <c r="W18" s="102"/>
       <c r="X18" s="5"/>
-      <c r="Y18" s="103"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y18" s="101"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B19" s="21"/>
-      <c r="C19" s="115"/>
+      <c r="C19" s="113"/>
       <c r="D19" s="26"/>
       <c r="E19" s="48"/>
       <c r="G19" s="76" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="76" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="O19" s="76"/>
       <c r="P19" s="5"/>
-      <c r="Q19" s="77"/>
-      <c r="S19" s="104"/>
+      <c r="Q19" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="S19" s="102"/>
       <c r="T19" s="5"/>
-      <c r="U19" s="103"/>
-      <c r="W19" s="104"/>
+      <c r="U19" s="101"/>
+      <c r="W19" s="102"/>
       <c r="X19" s="5"/>
-      <c r="Y19" s="103"/>
-    </row>
-    <row r="20" spans="1:25" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y19" s="101"/>
+    </row>
+    <row r="20" spans="1:25" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="60" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B20" s="61"/>
-      <c r="C20" s="114"/>
-      <c r="D20" s="62" t="s">
-        <v>51</v>
-      </c>
+      <c r="C20" s="112"/>
+      <c r="D20" s="62"/>
       <c r="E20" s="63"/>
       <c r="G20" s="78" t="s">
         <v>2</v>
       </c>
       <c r="H20" s="66"/>
-      <c r="I20" s="79" t="s">
-        <v>3</v>
+      <c r="I20" s="77" t="s">
+        <v>39</v>
       </c>
       <c r="J20" s="65"/>
       <c r="K20" s="78" t="s">
         <v>2</v>
       </c>
       <c r="L20" s="66"/>
-      <c r="M20" s="79" t="s">
-        <v>3</v>
+      <c r="M20" s="77" t="s">
+        <v>39</v>
       </c>
       <c r="O20" s="78" t="s">
         <v>2</v>
       </c>
       <c r="P20" s="66"/>
-      <c r="Q20" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="S20" s="105"/>
+      <c r="Q20" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="S20" s="103"/>
       <c r="T20" s="66"/>
-      <c r="U20" s="106"/>
-      <c r="W20" s="105"/>
+      <c r="U20" s="104"/>
+      <c r="W20" s="103"/>
       <c r="X20" s="66"/>
-      <c r="Y20" s="106"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y20" s="104"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B21" s="21"/>
-      <c r="C21" s="115" t="s">
-        <v>51</v>
-      </c>
+      <c r="C21" s="113"/>
       <c r="D21" s="26"/>
       <c r="E21" s="48"/>
       <c r="G21" s="76" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="76" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="77" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="O21" s="76"/>
       <c r="P21" s="5"/>
-      <c r="Q21" s="77"/>
-      <c r="S21" s="104"/>
+      <c r="Q21" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="S21" s="102"/>
       <c r="T21" s="5"/>
-      <c r="U21" s="103"/>
-      <c r="W21" s="104"/>
+      <c r="U21" s="101"/>
+      <c r="W21" s="102"/>
       <c r="X21" s="5"/>
-      <c r="Y21" s="103"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y21" s="101"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B22" s="21"/>
-      <c r="C22" s="115"/>
+      <c r="C22" s="113"/>
       <c r="D22" s="26"/>
       <c r="E22" s="48"/>
       <c r="G22" s="72" t="s">
         <v>0</v>
       </c>
       <c r="H22" s="6"/>
-      <c r="I22" s="73" t="s">
-        <v>3</v>
+      <c r="I22" s="77" t="s">
+        <v>39</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="72"/>
@@ -3532,22 +3535,22 @@
         <v>0</v>
       </c>
       <c r="P22" s="6"/>
-      <c r="Q22" s="73" t="s">
-        <v>3</v>
-      </c>
-      <c r="S22" s="98"/>
+      <c r="Q22" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="S22" s="96"/>
       <c r="T22" s="6"/>
-      <c r="U22" s="99"/>
-      <c r="W22" s="98"/>
+      <c r="U22" s="97"/>
+      <c r="W22" s="96"/>
       <c r="X22" s="6"/>
-      <c r="Y22" s="99"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y22" s="97"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B23" s="21"/>
-      <c r="C23" s="115"/>
+      <c r="C23" s="113"/>
       <c r="D23" s="26"/>
       <c r="E23" s="48"/>
       <c r="G23" s="72"/>
@@ -3560,37 +3563,37 @@
       <c r="O23" s="72"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="73"/>
-      <c r="S23" s="98"/>
+      <c r="S23" s="96"/>
       <c r="T23" s="6"/>
-      <c r="U23" s="99"/>
-      <c r="W23" s="98"/>
+      <c r="U23" s="97"/>
+      <c r="W23" s="96"/>
       <c r="X23" s="6"/>
-      <c r="Y23" s="99"/>
-    </row>
-    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y23" s="97"/>
+    </row>
+    <row r="24" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="24"/>
-      <c r="C24" s="116"/>
+      <c r="C24" s="114"/>
       <c r="D24" s="27"/>
       <c r="E24" s="49"/>
-      <c r="G24" s="82"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="84"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="82"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="82"/>
-      <c r="L24" s="83"/>
-      <c r="M24" s="84"/>
-      <c r="O24" s="82"/>
-      <c r="P24" s="83"/>
-      <c r="Q24" s="84"/>
-      <c r="S24" s="107"/>
-      <c r="T24" s="108"/>
-      <c r="U24" s="109"/>
-      <c r="W24" s="107"/>
-      <c r="X24" s="108"/>
-      <c r="Y24" s="109"/>
-    </row>
-    <row r="25" spans="1:25" ht="7.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K24" s="80"/>
+      <c r="L24" s="81"/>
+      <c r="M24" s="82"/>
+      <c r="O24" s="80"/>
+      <c r="P24" s="81"/>
+      <c r="Q24" s="82"/>
+      <c r="S24" s="105"/>
+      <c r="T24" s="106"/>
+      <c r="U24" s="107"/>
+      <c r="W24" s="105"/>
+      <c r="X24" s="106"/>
+      <c r="Y24" s="107"/>
+    </row>
+    <row r="25" spans="1:25" ht="7.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8"/>
       <c r="H25" s="1"/>
       <c r="I25" s="9"/>
@@ -3601,115 +3604,118 @@
       <c r="O25" s="8"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="9"/>
-      <c r="S25" s="93"/>
+      <c r="S25" s="91"/>
       <c r="T25" s="2"/>
-      <c r="U25" s="94"/>
+      <c r="U25" s="92"/>
       <c r="W25" s="8"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="9"/>
     </row>
-    <row r="26" spans="1:25" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="52" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
-      <c r="G26" s="130" t="s">
-        <v>58</v>
-      </c>
-      <c r="H26" s="131"/>
-      <c r="I26" s="132"/>
+      <c r="G26" s="138" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" s="139"/>
+      <c r="I26" s="140"/>
       <c r="J26" s="17"/>
-      <c r="K26" s="130" t="s">
-        <v>59</v>
-      </c>
-      <c r="L26" s="131"/>
-      <c r="M26" s="132"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="130" t="s">
-        <v>60</v>
-      </c>
-      <c r="P26" s="131"/>
-      <c r="Q26" s="132"/>
+      <c r="K26" s="138" t="s">
+        <v>55</v>
+      </c>
+      <c r="L26" s="139"/>
+      <c r="M26" s="140"/>
+      <c r="N26" s="17" t="e">
+        <f>fieldType</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O26" s="138" t="s">
+        <v>56</v>
+      </c>
+      <c r="P26" s="139"/>
+      <c r="Q26" s="140"/>
       <c r="R26" s="17"/>
-      <c r="S26" s="123" t="s">
-        <v>61</v>
-      </c>
-      <c r="T26" s="124"/>
-      <c r="U26" s="125"/>
+      <c r="S26" s="131" t="s">
+        <v>57</v>
+      </c>
+      <c r="T26" s="132"/>
+      <c r="U26" s="133"/>
       <c r="V26" s="17"/>
-      <c r="W26" s="123" t="s">
-        <v>61</v>
-      </c>
-      <c r="X26" s="124"/>
-      <c r="Y26" s="125"/>
-    </row>
-    <row r="27" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W26" s="131" t="s">
+        <v>57</v>
+      </c>
+      <c r="X26" s="132"/>
+      <c r="Y26" s="133"/>
+    </row>
+    <row r="27" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="53" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" s="54" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="54" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G27" s="69" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H27" s="70" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I27" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="L27" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="K27" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="L27" s="70" t="s">
-        <v>32</v>
-      </c>
       <c r="M27" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="O27" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="P27" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="O27" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="P27" s="70" t="s">
-        <v>32</v>
-      </c>
       <c r="Q27" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="S27" s="115" t="s">
+        <v>27</v>
+      </c>
+      <c r="T27" s="116" t="s">
         <v>30</v>
       </c>
-      <c r="S27" s="117" t="s">
-        <v>29</v>
-      </c>
-      <c r="T27" s="118" t="s">
-        <v>32</v>
-      </c>
-      <c r="U27" s="119" t="s">
+      <c r="U27" s="117" t="s">
+        <v>28</v>
+      </c>
+      <c r="W27" s="115" t="s">
+        <v>27</v>
+      </c>
+      <c r="X27" s="116" t="s">
         <v>30</v>
       </c>
-      <c r="W27" s="117" t="s">
-        <v>29</v>
-      </c>
-      <c r="X27" s="118" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y27" s="119" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Y27" s="117" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C28" s="36"/>
       <c r="D28" s="30"/>
@@ -3717,7 +3723,7 @@
       <c r="G28" s="76"/>
       <c r="H28" s="5"/>
       <c r="I28" s="77" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K28" s="76"/>
       <c r="L28" s="5"/>
@@ -3725,19 +3731,19 @@
       <c r="O28" s="76"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="77"/>
-      <c r="S28" s="104"/>
+      <c r="S28" s="102"/>
       <c r="T28" s="5"/>
-      <c r="U28" s="103"/>
-      <c r="W28" s="104"/>
+      <c r="U28" s="101"/>
+      <c r="W28" s="102"/>
       <c r="X28" s="5"/>
-      <c r="Y28" s="103"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y28" s="101"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" s="37"/>
       <c r="D29" s="31"/>
@@ -3745,7 +3751,7 @@
       <c r="G29" s="76"/>
       <c r="H29" s="5"/>
       <c r="I29" s="77" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K29" s="76"/>
       <c r="L29" s="5"/>
@@ -3753,19 +3759,19 @@
       <c r="O29" s="76"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="77"/>
-      <c r="S29" s="104"/>
+      <c r="S29" s="102"/>
       <c r="T29" s="5"/>
-      <c r="U29" s="103"/>
-      <c r="W29" s="104"/>
+      <c r="U29" s="101"/>
+      <c r="W29" s="102"/>
       <c r="X29" s="5"/>
-      <c r="Y29" s="103"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y29" s="101"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C30" s="37"/>
       <c r="D30" s="31"/>
@@ -3779,19 +3785,19 @@
       <c r="O30" s="76"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="77"/>
-      <c r="S30" s="104"/>
+      <c r="S30" s="102"/>
       <c r="T30" s="5"/>
-      <c r="U30" s="103"/>
-      <c r="W30" s="104"/>
+      <c r="U30" s="101"/>
+      <c r="W30" s="102"/>
       <c r="X30" s="5"/>
-      <c r="Y30" s="103"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y30" s="101"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31" s="37"/>
       <c r="D31" s="31"/>
@@ -3805,16 +3811,16 @@
       <c r="O31" s="76"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="77"/>
-      <c r="S31" s="104"/>
+      <c r="S31" s="102"/>
       <c r="T31" s="5"/>
-      <c r="U31" s="103"/>
-      <c r="W31" s="104"/>
+      <c r="U31" s="101"/>
+      <c r="W31" s="102"/>
       <c r="X31" s="5"/>
-      <c r="Y31" s="103"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y31" s="101"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B32" s="31"/>
       <c r="C32" s="37"/>
@@ -3829,16 +3835,16 @@
       <c r="O32" s="76"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="77"/>
-      <c r="S32" s="104"/>
+      <c r="S32" s="102"/>
       <c r="T32" s="5"/>
-      <c r="U32" s="103"/>
-      <c r="W32" s="104"/>
+      <c r="U32" s="101"/>
+      <c r="W32" s="102"/>
       <c r="X32" s="5"/>
-      <c r="Y32" s="103"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y32" s="101"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B33" s="31"/>
       <c r="C33" s="37"/>
@@ -3853,16 +3859,16 @@
       <c r="O33" s="76"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="77"/>
-      <c r="S33" s="104"/>
+      <c r="S33" s="102"/>
       <c r="T33" s="5"/>
-      <c r="U33" s="103"/>
-      <c r="W33" s="104"/>
+      <c r="U33" s="101"/>
+      <c r="W33" s="102"/>
       <c r="X33" s="5"/>
-      <c r="Y33" s="103"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y33" s="101"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B34" s="31"/>
       <c r="C34" s="37"/>
@@ -3877,16 +3883,16 @@
       <c r="O34" s="76"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="77"/>
-      <c r="S34" s="104"/>
+      <c r="S34" s="102"/>
       <c r="T34" s="5"/>
-      <c r="U34" s="103"/>
-      <c r="W34" s="104"/>
+      <c r="U34" s="101"/>
+      <c r="W34" s="102"/>
       <c r="X34" s="5"/>
-      <c r="Y34" s="103"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y34" s="101"/>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B35" s="31"/>
       <c r="C35" s="37"/>
@@ -3901,16 +3907,16 @@
       <c r="O35" s="76"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="77"/>
-      <c r="S35" s="104"/>
+      <c r="S35" s="102"/>
       <c r="T35" s="5"/>
-      <c r="U35" s="103"/>
-      <c r="W35" s="104"/>
+      <c r="U35" s="101"/>
+      <c r="W35" s="102"/>
       <c r="X35" s="5"/>
-      <c r="Y35" s="103"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y35" s="101"/>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B36" s="31"/>
       <c r="C36" s="37"/>
@@ -3925,98 +3931,98 @@
       <c r="O36" s="76"/>
       <c r="P36" s="5"/>
       <c r="Q36" s="77"/>
-      <c r="S36" s="104"/>
+      <c r="S36" s="102"/>
       <c r="T36" s="5"/>
-      <c r="U36" s="103"/>
-      <c r="W36" s="104"/>
+      <c r="U36" s="101"/>
+      <c r="W36" s="102"/>
       <c r="X36" s="5"/>
-      <c r="Y36" s="103"/>
-    </row>
-    <row r="37" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y36" s="101"/>
+    </row>
+    <row r="37" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B37" s="32"/>
       <c r="C37" s="38"/>
       <c r="D37" s="32"/>
       <c r="E37" s="46"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="84"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="82"/>
       <c r="K37" s="72"/>
       <c r="L37" s="6"/>
       <c r="M37" s="73"/>
-      <c r="O37" s="82"/>
-      <c r="P37" s="83"/>
-      <c r="Q37" s="84"/>
-      <c r="S37" s="98"/>
+      <c r="O37" s="80"/>
+      <c r="P37" s="81"/>
+      <c r="Q37" s="82"/>
+      <c r="S37" s="96"/>
       <c r="T37" s="6"/>
-      <c r="U37" s="99"/>
-      <c r="W37" s="98"/>
+      <c r="U37" s="97"/>
+      <c r="W37" s="96"/>
       <c r="X37" s="6"/>
-      <c r="Y37" s="99"/>
-    </row>
-    <row r="38" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y37" s="97"/>
+    </row>
+    <row r="38" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G38" s="69" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H38" s="70" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I38" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="K38" s="83" t="s">
+        <v>27</v>
+      </c>
+      <c r="L38" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="K38" s="85" t="s">
-        <v>29</v>
-      </c>
-      <c r="L38" s="86" t="s">
-        <v>32</v>
-      </c>
-      <c r="M38" s="87" t="s">
+      <c r="M38" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="O38" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="P38" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="O38" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="P38" s="70" t="s">
-        <v>32</v>
-      </c>
       <c r="Q38" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="S38" s="109" t="s">
+        <v>27</v>
+      </c>
+      <c r="T38" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="S38" s="111" t="s">
-        <v>29</v>
-      </c>
-      <c r="T38" s="110" t="s">
-        <v>32</v>
-      </c>
-      <c r="U38" s="112" t="s">
+      <c r="U38" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="W38" s="109" t="s">
+        <v>27</v>
+      </c>
+      <c r="X38" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="W38" s="111" t="s">
-        <v>29</v>
-      </c>
-      <c r="X38" s="110" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y38" s="112" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Y38" s="110" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A39" s="29" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B39" s="30"/>
       <c r="C39" s="36"/>
@@ -4025,22 +4031,22 @@
       <c r="G39" s="76"/>
       <c r="H39" s="5"/>
       <c r="I39" s="77"/>
-      <c r="K39" s="88"/>
+      <c r="K39" s="86"/>
       <c r="L39" s="5"/>
-      <c r="M39" s="89"/>
+      <c r="M39" s="87"/>
       <c r="O39" s="76"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="77"/>
-      <c r="S39" s="104"/>
+      <c r="S39" s="102"/>
       <c r="T39" s="5"/>
-      <c r="U39" s="103"/>
-      <c r="W39" s="104"/>
+      <c r="U39" s="101"/>
+      <c r="W39" s="102"/>
       <c r="X39" s="5"/>
-      <c r="Y39" s="103"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y39" s="101"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B40" s="31"/>
       <c r="C40" s="37"/>
@@ -4049,22 +4055,22 @@
       <c r="G40" s="76"/>
       <c r="H40" s="5"/>
       <c r="I40" s="77"/>
-      <c r="K40" s="88"/>
+      <c r="K40" s="86"/>
       <c r="L40" s="5"/>
-      <c r="M40" s="89"/>
+      <c r="M40" s="87"/>
       <c r="O40" s="76"/>
       <c r="P40" s="5"/>
       <c r="Q40" s="77"/>
-      <c r="S40" s="104"/>
+      <c r="S40" s="102"/>
       <c r="T40" s="5"/>
-      <c r="U40" s="103"/>
-      <c r="W40" s="104"/>
+      <c r="U40" s="101"/>
+      <c r="W40" s="102"/>
       <c r="X40" s="5"/>
-      <c r="Y40" s="103"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y40" s="101"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B41" s="31"/>
       <c r="C41" s="37"/>
@@ -4073,22 +4079,22 @@
       <c r="G41" s="76"/>
       <c r="H41" s="5"/>
       <c r="I41" s="77"/>
-      <c r="K41" s="88"/>
+      <c r="K41" s="86"/>
       <c r="L41" s="5"/>
-      <c r="M41" s="89"/>
+      <c r="M41" s="87"/>
       <c r="O41" s="76"/>
       <c r="P41" s="5"/>
       <c r="Q41" s="77"/>
-      <c r="S41" s="104"/>
+      <c r="S41" s="102"/>
       <c r="T41" s="5"/>
-      <c r="U41" s="103"/>
-      <c r="W41" s="104"/>
+      <c r="U41" s="101"/>
+      <c r="W41" s="102"/>
       <c r="X41" s="5"/>
-      <c r="Y41" s="103"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y41" s="101"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B42" s="31"/>
       <c r="C42" s="37"/>
@@ -4097,22 +4103,22 @@
       <c r="G42" s="76"/>
       <c r="H42" s="5"/>
       <c r="I42" s="77"/>
-      <c r="K42" s="88"/>
+      <c r="K42" s="86"/>
       <c r="L42" s="5"/>
-      <c r="M42" s="89"/>
+      <c r="M42" s="87"/>
       <c r="O42" s="76"/>
       <c r="P42" s="5"/>
       <c r="Q42" s="77"/>
-      <c r="S42" s="104"/>
+      <c r="S42" s="102"/>
       <c r="T42" s="5"/>
-      <c r="U42" s="103"/>
-      <c r="W42" s="104"/>
+      <c r="U42" s="101"/>
+      <c r="W42" s="102"/>
       <c r="X42" s="5"/>
-      <c r="Y42" s="103"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y42" s="101"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B43" s="31"/>
       <c r="C43" s="37"/>
@@ -4121,22 +4127,22 @@
       <c r="G43" s="76"/>
       <c r="H43" s="5"/>
       <c r="I43" s="77"/>
-      <c r="K43" s="88"/>
+      <c r="K43" s="86"/>
       <c r="L43" s="5"/>
-      <c r="M43" s="89"/>
+      <c r="M43" s="87"/>
       <c r="O43" s="76"/>
       <c r="P43" s="5"/>
       <c r="Q43" s="77"/>
-      <c r="S43" s="104"/>
+      <c r="S43" s="102"/>
       <c r="T43" s="5"/>
-      <c r="U43" s="103"/>
-      <c r="W43" s="104"/>
+      <c r="U43" s="101"/>
+      <c r="W43" s="102"/>
       <c r="X43" s="5"/>
-      <c r="Y43" s="103"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y43" s="101"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B44" s="31"/>
       <c r="C44" s="37"/>
@@ -4145,22 +4151,22 @@
       <c r="G44" s="76"/>
       <c r="H44" s="5"/>
       <c r="I44" s="77"/>
-      <c r="K44" s="88"/>
+      <c r="K44" s="86"/>
       <c r="L44" s="5"/>
-      <c r="M44" s="89"/>
+      <c r="M44" s="87"/>
       <c r="O44" s="76"/>
       <c r="P44" s="5"/>
       <c r="Q44" s="77"/>
-      <c r="S44" s="104"/>
+      <c r="S44" s="102"/>
       <c r="T44" s="5"/>
-      <c r="U44" s="103"/>
-      <c r="W44" s="104"/>
+      <c r="U44" s="101"/>
+      <c r="W44" s="102"/>
       <c r="X44" s="5"/>
-      <c r="Y44" s="103"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y44" s="101"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B45" s="31"/>
       <c r="C45" s="37"/>
@@ -4169,22 +4175,22 @@
       <c r="G45" s="76"/>
       <c r="H45" s="5"/>
       <c r="I45" s="77"/>
-      <c r="K45" s="88"/>
+      <c r="K45" s="86"/>
       <c r="L45" s="5"/>
-      <c r="M45" s="89"/>
+      <c r="M45" s="87"/>
       <c r="O45" s="76"/>
       <c r="P45" s="5"/>
       <c r="Q45" s="77"/>
-      <c r="S45" s="104"/>
+      <c r="S45" s="102"/>
       <c r="T45" s="5"/>
-      <c r="U45" s="103"/>
-      <c r="W45" s="104"/>
+      <c r="U45" s="101"/>
+      <c r="W45" s="102"/>
       <c r="X45" s="5"/>
-      <c r="Y45" s="103"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y45" s="101"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B46" s="31"/>
       <c r="C46" s="37"/>
@@ -4193,22 +4199,22 @@
       <c r="G46" s="76"/>
       <c r="H46" s="5"/>
       <c r="I46" s="77"/>
-      <c r="K46" s="88"/>
+      <c r="K46" s="86"/>
       <c r="L46" s="5"/>
-      <c r="M46" s="89"/>
+      <c r="M46" s="87"/>
       <c r="O46" s="76"/>
       <c r="P46" s="5"/>
       <c r="Q46" s="77"/>
-      <c r="S46" s="104"/>
+      <c r="S46" s="102"/>
       <c r="T46" s="5"/>
-      <c r="U46" s="103"/>
-      <c r="W46" s="104"/>
+      <c r="U46" s="101"/>
+      <c r="W46" s="102"/>
       <c r="X46" s="5"/>
-      <c r="Y46" s="103"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y46" s="101"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B47" s="31"/>
       <c r="C47" s="37"/>
@@ -4217,117 +4223,117 @@
       <c r="G47" s="76"/>
       <c r="H47" s="5"/>
       <c r="I47" s="77"/>
-      <c r="K47" s="88"/>
+      <c r="K47" s="86"/>
       <c r="L47" s="5"/>
-      <c r="M47" s="89"/>
+      <c r="M47" s="87"/>
       <c r="O47" s="76"/>
       <c r="P47" s="5"/>
       <c r="Q47" s="77"/>
-      <c r="S47" s="104"/>
+      <c r="S47" s="102"/>
       <c r="T47" s="5"/>
-      <c r="U47" s="103"/>
-      <c r="W47" s="104"/>
+      <c r="U47" s="101"/>
+      <c r="W47" s="102"/>
       <c r="X47" s="5"/>
-      <c r="Y47" s="103"/>
-    </row>
-    <row r="48" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y47" s="101"/>
+    </row>
+    <row r="48" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B48" s="32"/>
       <c r="C48" s="38"/>
       <c r="D48" s="32"/>
       <c r="E48" s="46"/>
-      <c r="G48" s="82"/>
-      <c r="H48" s="83"/>
-      <c r="I48" s="84"/>
-      <c r="K48" s="90"/>
-      <c r="L48" s="91"/>
-      <c r="M48" s="92"/>
-      <c r="O48" s="82"/>
-      <c r="P48" s="83"/>
-      <c r="Q48" s="84"/>
-      <c r="S48" s="107"/>
-      <c r="T48" s="108"/>
-      <c r="U48" s="109"/>
-      <c r="W48" s="107"/>
-      <c r="X48" s="108"/>
-      <c r="Y48" s="109"/>
-    </row>
-    <row r="49" spans="1:25" ht="7.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G48" s="80"/>
+      <c r="H48" s="81"/>
+      <c r="I48" s="82"/>
+      <c r="K48" s="88"/>
+      <c r="L48" s="89"/>
+      <c r="M48" s="90"/>
+      <c r="O48" s="80"/>
+      <c r="P48" s="81"/>
+      <c r="Q48" s="82"/>
+      <c r="S48" s="105"/>
+      <c r="T48" s="106"/>
+      <c r="U48" s="107"/>
+      <c r="W48" s="105"/>
+      <c r="X48" s="106"/>
+      <c r="Y48" s="107"/>
+    </row>
+    <row r="49" spans="1:25" ht="7.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G50" s="69" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H50" s="70" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I50" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="K50" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="L50" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="K50" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="L50" s="70" t="s">
-        <v>32</v>
-      </c>
       <c r="M50" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="O50" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="P50" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="O50" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="P50" s="70" t="s">
-        <v>32</v>
-      </c>
       <c r="Q50" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="S50" s="109" t="s">
+        <v>27</v>
+      </c>
+      <c r="T50" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="S50" s="111" t="s">
-        <v>29</v>
-      </c>
-      <c r="T50" s="110" t="s">
-        <v>32</v>
-      </c>
-      <c r="U50" s="112" t="s">
+      <c r="U50" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="W50" s="109" t="s">
+        <v>27</v>
+      </c>
+      <c r="X50" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="W50" s="111" t="s">
-        <v>29</v>
-      </c>
-      <c r="X50" s="110" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y50" s="112" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Y50" s="110" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A51" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B51" s="133" t="s">
-        <v>93</v>
-      </c>
-      <c r="C51" s="134"/>
-      <c r="D51" s="135"/>
+        <v>85</v>
+      </c>
+      <c r="B51" s="125" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="126"/>
+      <c r="D51" s="127"/>
       <c r="E51" s="41"/>
       <c r="G51" s="76"/>
       <c r="H51" s="5"/>
@@ -4338,22 +4344,22 @@
       <c r="O51" s="76"/>
       <c r="P51" s="5"/>
       <c r="Q51" s="77"/>
-      <c r="S51" s="104"/>
+      <c r="S51" s="102"/>
       <c r="T51" s="5"/>
-      <c r="U51" s="103"/>
-      <c r="W51" s="104"/>
+      <c r="U51" s="101"/>
+      <c r="W51" s="102"/>
       <c r="X51" s="5"/>
-      <c r="Y51" s="103"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y51" s="101"/>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A52" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B52" s="136" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" s="137"/>
-      <c r="D52" s="138"/>
+        <v>87</v>
+      </c>
+      <c r="B52" s="119" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="120"/>
+      <c r="D52" s="121"/>
       <c r="E52" s="42"/>
       <c r="G52" s="76"/>
       <c r="H52" s="5"/>
@@ -4364,22 +4370,22 @@
       <c r="O52" s="76"/>
       <c r="P52" s="5"/>
       <c r="Q52" s="77"/>
-      <c r="S52" s="104"/>
+      <c r="S52" s="102"/>
       <c r="T52" s="5"/>
-      <c r="U52" s="103"/>
-      <c r="W52" s="104"/>
+      <c r="U52" s="101"/>
+      <c r="W52" s="102"/>
       <c r="X52" s="5"/>
-      <c r="Y52" s="103"/>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y52" s="101"/>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A53" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="B53" s="136" t="s">
-        <v>97</v>
-      </c>
-      <c r="C53" s="137"/>
-      <c r="D53" s="138"/>
+        <v>89</v>
+      </c>
+      <c r="B53" s="119" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="120"/>
+      <c r="D53" s="121"/>
       <c r="E53" s="42"/>
       <c r="G53" s="76"/>
       <c r="H53" s="5"/>
@@ -4390,22 +4396,22 @@
       <c r="O53" s="76"/>
       <c r="P53" s="5"/>
       <c r="Q53" s="77"/>
-      <c r="S53" s="104"/>
+      <c r="S53" s="102"/>
       <c r="T53" s="5"/>
-      <c r="U53" s="103"/>
-      <c r="W53" s="104"/>
+      <c r="U53" s="101"/>
+      <c r="W53" s="102"/>
       <c r="X53" s="5"/>
-      <c r="Y53" s="103"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y53" s="101"/>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A54" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="B54" s="136" t="s">
-        <v>99</v>
-      </c>
-      <c r="C54" s="137"/>
-      <c r="D54" s="138"/>
+        <v>91</v>
+      </c>
+      <c r="B54" s="119" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="120"/>
+      <c r="D54" s="121"/>
       <c r="E54" s="42"/>
       <c r="G54" s="76"/>
       <c r="H54" s="5"/>
@@ -4416,33 +4422,33 @@
       <c r="O54" s="76"/>
       <c r="P54" s="5"/>
       <c r="Q54" s="77"/>
-      <c r="S54" s="104"/>
+      <c r="S54" s="102"/>
       <c r="T54" s="5"/>
-      <c r="U54" s="103"/>
-      <c r="W54" s="104"/>
+      <c r="U54" s="101"/>
+      <c r="W54" s="102"/>
       <c r="X54" s="5"/>
-      <c r="Y54" s="103"/>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y54" s="101"/>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A55" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="B55" s="136" t="s">
-        <v>52</v>
-      </c>
-      <c r="C55" s="137"/>
-      <c r="D55" s="138"/>
+        <v>93</v>
+      </c>
+      <c r="B55" s="119" t="s">
+        <v>49</v>
+      </c>
+      <c r="C55" s="120"/>
+      <c r="D55" s="121"/>
       <c r="E55" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G55" s="76" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I55" s="77" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="K55" s="76"/>
       <c r="L55" s="5"/>
@@ -4450,14 +4456,14 @@
       <c r="O55" s="76"/>
       <c r="P55" s="5"/>
       <c r="Q55" s="77"/>
-      <c r="S55" s="104"/>
+      <c r="S55" s="102"/>
       <c r="T55" s="5"/>
-      <c r="U55" s="103"/>
-      <c r="W55" s="104"/>
+      <c r="U55" s="101"/>
+      <c r="W55" s="102"/>
       <c r="X55" s="5"/>
-      <c r="Y55" s="103"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y55" s="101"/>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A56" s="34"/>
       <c r="B56" s="55"/>
       <c r="C56" s="56"/>
@@ -4472,18 +4478,18 @@
       <c r="O56" s="76"/>
       <c r="P56" s="5"/>
       <c r="Q56" s="77"/>
-      <c r="S56" s="104"/>
+      <c r="S56" s="102"/>
       <c r="T56" s="5"/>
-      <c r="U56" s="103"/>
-      <c r="W56" s="104"/>
+      <c r="U56" s="101"/>
+      <c r="W56" s="102"/>
       <c r="X56" s="5"/>
-      <c r="Y56" s="103"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y56" s="101"/>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A57" s="34"/>
-      <c r="B57" s="136"/>
-      <c r="C57" s="137"/>
-      <c r="D57" s="138"/>
+      <c r="B57" s="119"/>
+      <c r="C57" s="120"/>
+      <c r="D57" s="121"/>
       <c r="E57" s="42"/>
       <c r="G57" s="76"/>
       <c r="H57" s="5"/>
@@ -4494,18 +4500,18 @@
       <c r="O57" s="76"/>
       <c r="P57" s="5"/>
       <c r="Q57" s="77"/>
-      <c r="S57" s="104"/>
+      <c r="S57" s="102"/>
       <c r="T57" s="5"/>
-      <c r="U57" s="103"/>
-      <c r="W57" s="104"/>
+      <c r="U57" s="101"/>
+      <c r="W57" s="102"/>
       <c r="X57" s="5"/>
-      <c r="Y57" s="103"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y57" s="101"/>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A58" s="34"/>
-      <c r="B58" s="136"/>
-      <c r="C58" s="137"/>
-      <c r="D58" s="138"/>
+      <c r="B58" s="119"/>
+      <c r="C58" s="120"/>
+      <c r="D58" s="121"/>
       <c r="E58" s="42"/>
       <c r="G58" s="76"/>
       <c r="H58" s="5"/>
@@ -4516,18 +4522,18 @@
       <c r="O58" s="76"/>
       <c r="P58" s="5"/>
       <c r="Q58" s="77"/>
-      <c r="S58" s="104"/>
+      <c r="S58" s="102"/>
       <c r="T58" s="5"/>
-      <c r="U58" s="103"/>
-      <c r="W58" s="104"/>
+      <c r="U58" s="101"/>
+      <c r="W58" s="102"/>
       <c r="X58" s="5"/>
-      <c r="Y58" s="103"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y58" s="101"/>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A59" s="34"/>
-      <c r="B59" s="136"/>
-      <c r="C59" s="137"/>
-      <c r="D59" s="138"/>
+      <c r="B59" s="119"/>
+      <c r="C59" s="120"/>
+      <c r="D59" s="121"/>
       <c r="E59" s="42"/>
       <c r="G59" s="76"/>
       <c r="H59" s="5"/>
@@ -4538,18 +4544,18 @@
       <c r="O59" s="76"/>
       <c r="P59" s="5"/>
       <c r="Q59" s="77"/>
-      <c r="S59" s="104"/>
+      <c r="S59" s="102"/>
       <c r="T59" s="5"/>
-      <c r="U59" s="103"/>
-      <c r="W59" s="104"/>
+      <c r="U59" s="101"/>
+      <c r="W59" s="102"/>
       <c r="X59" s="5"/>
-      <c r="Y59" s="103"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y59" s="101"/>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A60" s="34"/>
-      <c r="B60" s="136"/>
-      <c r="C60" s="137"/>
-      <c r="D60" s="138"/>
+      <c r="B60" s="119"/>
+      <c r="C60" s="120"/>
+      <c r="D60" s="121"/>
       <c r="E60" s="42"/>
       <c r="G60" s="76"/>
       <c r="H60" s="5"/>
@@ -4560,59 +4566,50 @@
       <c r="O60" s="76"/>
       <c r="P60" s="5"/>
       <c r="Q60" s="77"/>
-      <c r="S60" s="104"/>
+      <c r="S60" s="102"/>
       <c r="T60" s="5"/>
-      <c r="U60" s="103"/>
-      <c r="W60" s="104"/>
+      <c r="U60" s="101"/>
+      <c r="W60" s="102"/>
       <c r="X60" s="5"/>
-      <c r="Y60" s="103"/>
-    </row>
-    <row r="61" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y60" s="101"/>
+    </row>
+    <row r="61" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="35"/>
-      <c r="B61" s="139"/>
-      <c r="C61" s="140"/>
-      <c r="D61" s="141"/>
+      <c r="B61" s="122"/>
+      <c r="C61" s="123"/>
+      <c r="D61" s="124"/>
       <c r="E61" s="43"/>
-      <c r="G61" s="82"/>
-      <c r="H61" s="83"/>
-      <c r="I61" s="84"/>
-      <c r="K61" s="82"/>
-      <c r="L61" s="83"/>
-      <c r="M61" s="84"/>
-      <c r="O61" s="82"/>
-      <c r="P61" s="83"/>
-      <c r="Q61" s="84"/>
-      <c r="S61" s="107"/>
-      <c r="T61" s="108"/>
-      <c r="U61" s="109"/>
-      <c r="W61" s="107"/>
-      <c r="X61" s="108"/>
-      <c r="Y61" s="109"/>
-    </row>
-    <row r="62" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="G61" s="80"/>
+      <c r="H61" s="81"/>
+      <c r="I61" s="82"/>
+      <c r="K61" s="80"/>
+      <c r="L61" s="81"/>
+      <c r="M61" s="82"/>
+      <c r="O61" s="80"/>
+      <c r="P61" s="81"/>
+      <c r="Q61" s="82"/>
+      <c r="S61" s="105"/>
+      <c r="T61" s="106"/>
+      <c r="U61" s="107"/>
+      <c r="W61" s="105"/>
+      <c r="X61" s="106"/>
+      <c r="Y61" s="107"/>
+    </row>
+    <row r="62" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="c8EEcgg7c/OT6veU/C3xWZbRprRxXTGRlRDOOnMXwDGvoWL6JOeB1maVWmy1Xw1auZ6GVMf1iSDLpYVZbPMLvw==" saltValue="fLEZ+YE5W3cU2B+blIZxXg==" spinCount="100000" sheet="1" insertColumns="0" insertRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="boxHoXBX34oUrLUM+h6Wl+v1yk0Mbc8Hmvviu4+faSLpfMLPm7RW8r+t1/6EAnPNbmhwbUKnmUg10Y5G+TRFzw==" saltValue="FOp4u7R0PjClGdxDUddDxQ==" spinCount="100000" sheet="1" insertColumns="0" insertRows="0"/>
   <protectedRanges>
+    <protectedRange sqref="S4:Y61" name="customEntities"/>
+    <protectedRange sqref="A51:D55" name="Questionnaire_3"/>
+    <protectedRange sqref="A39:A48" name="Questionnaire_2"/>
+    <protectedRange sqref="A28:A37" name="Questionnaire_1"/>
+    <protectedRange sqref="B8:B12" name="Contact Fields_2"/>
+    <protectedRange sqref="A8:A23" name="Contact Fields_1"/>
+    <protectedRange sqref="B28:Y37 B39:Y48 A56:Y61 A38:E38 E51:Y55" name="Questionnaire"/>
+    <protectedRange sqref="A7:Y7 A24:Y24 B23:Y23 C8:Y8 B13:H22 C9:H12 I9:Y22" name="Contact Fields"/>
     <protectedRange sqref="A1" name="Titel"/>
-    <protectedRange sqref="A7:Y7 A24:Y24 B13:Y23 C8:Y12" name="Contact Fields"/>
-    <protectedRange sqref="B28:Y37 B39:Y48 A56:Y61 A38:E38 E51:Y55" name="Questionnaire"/>
-    <protectedRange sqref="A8:A23" name="Contact Fields_1"/>
-    <protectedRange sqref="B8:B12" name="Contact Fields_2"/>
-    <protectedRange sqref="A28:A37" name="Questionnaire_1"/>
-    <protectedRange sqref="A39:A48" name="Questionnaire_2"/>
-    <protectedRange sqref="A51:D55" name="Questionnaire_3"/>
   </protectedRanges>
   <mergeCells count="20">
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="S26:U26"/>
     <mergeCell ref="W4:Y4"/>
@@ -4623,17 +4620,35 @@
     <mergeCell ref="K26:M26"/>
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="O26:Q26"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A24:AG27 B13:AG23 C8:AG12 A38:AG38 B28:AG37 B39:AG48">
-    <cfRule type="expression" dxfId="19" priority="19">
+  <conditionalFormatting sqref="A24:AG27 A38:AG38 B28:AG37 B39:AG48 I9:I22 C8:AG11 B23:AG23 B13:P22 C12:P12 R12:AG22">
+    <cfRule type="expression" dxfId="21" priority="21">
       <formula>$C8="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="20">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>$D8="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W51:Y61">
+    <cfRule type="expression" dxfId="19" priority="19">
+      <formula>$C51="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="20">
+      <formula>$D51="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S51:U61">
     <cfRule type="expression" dxfId="17" priority="17">
       <formula>$C51="x"</formula>
     </cfRule>
@@ -4641,7 +4656,7 @@
       <formula>$D51="x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S51:U61">
+  <conditionalFormatting sqref="O51:Q61">
     <cfRule type="expression" dxfId="15" priority="15">
       <formula>$C51="x"</formula>
     </cfRule>
@@ -4649,7 +4664,7 @@
       <formula>$D51="x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O51:Q61">
+  <conditionalFormatting sqref="K51:M61">
     <cfRule type="expression" dxfId="13" priority="13">
       <formula>$C51="x"</formula>
     </cfRule>
@@ -4657,7 +4672,7 @@
       <formula>$D51="x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K51:M61">
+  <conditionalFormatting sqref="G51:I61">
     <cfRule type="expression" dxfId="11" priority="11">
       <formula>$C51="x"</formula>
     </cfRule>
@@ -4665,15 +4680,15 @@
       <formula>$D51="x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G51:I61">
+  <conditionalFormatting sqref="A8:A23">
     <cfRule type="expression" dxfId="9" priority="9">
-      <formula>$C51="x"</formula>
+      <formula>$C8="x"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="8" priority="10">
-      <formula>$D51="x"</formula>
+      <formula>$D8="x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:A23">
+  <conditionalFormatting sqref="B8:B12">
     <cfRule type="expression" dxfId="7" priority="7">
       <formula>$C8="x"</formula>
     </cfRule>
@@ -4681,30 +4696,38 @@
       <formula>$D8="x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B12">
+  <conditionalFormatting sqref="A28:A37">
     <cfRule type="expression" dxfId="5" priority="5">
-      <formula>$C8="x"</formula>
+      <formula>$C28="x"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
-      <formula>$D8="x"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28:A37">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>$C28="x"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$D28="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:A48">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$C39="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$D39="x"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Q12:Q22">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$C12="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$D12="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D24 C28:D37 C39:D48" xr:uid="{7904A3F4-6221-4D64-AD0E-1F4168BBF862}">
+      <formula1>"x"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M39:M48 I7:I24 M7:M24 U7:U24 Y7:Y24 Y28:Y37 U28:U37 Q28:Q37 M28:M37 I28:I37 I39:I48 Q39:Q48 U39:U48 Y39:Y48 Y51:Y61 U51:U61 Q51:Q61 M51:M61 I51:I61 Q7:Q24" xr:uid="{602B57E5-9BC3-430C-9CF1-45F2FF9C756D}">
+      <formula1>"text, boolean, number, picklist, multipicklist, lookup"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -4712,21 +4735,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010060A44420B6B801499790497461B7617A" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fabbcee23a04d27af1ae9e54f4461bef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8f774076-1ef3-4740-8929-5969f04599b3" xmlns:ns4="8b2a92f5-6e7f-40fd-b6fe-382c9779cf32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c03e0335abb4116b770311e5abaeb524" ns3:_="" ns4:_="">
     <xsd:import namespace="8f774076-1ef3-4740-8929-5969f04599b3"/>
@@ -4935,32 +4943,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B94D2B0B-0398-4829-B93A-C49C0FAED7B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDAAE1C4-DB1B-4159-B8B9-55C0242E8521}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="8b2a92f5-6e7f-40fd-b6fe-382c9779cf32"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8f774076-1ef3-4740-8929-5969f04599b3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4CDBC7-0A6E-420D-A4CD-91BDFDE80302}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4977,4 +4975,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDAAE1C4-DB1B-4159-B8B9-55C0242E8521}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8b2a92f5-6e7f-40fd-b6fe-382c9779cf32"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8f774076-1ef3-4740-8929-5969f04599b3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B94D2B0B-0398-4829-B93A-C49C0FAED7B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>